<commit_message>
chg: Updated Ordnance for D7.2
</commit_message>
<xml_diff>
--- a/ORDERS/JFACC/OPAR JFACC Standard Conventional Loads.xlsx
+++ b/ORDERS/JFACC/OPAR JFACC Standard Conventional Loads.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minda\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53269913-E0B8-4CC4-A5B9-98B888CF0C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DEC65332-D3F4-43F9-A75C-C1DCC099597E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="A-10C2" sheetId="3" r:id="rId1"/>
@@ -25,9 +19,9 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'F-16'!$A$1:$K$60</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'F-18C'!$A$1:$I$51</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -637,9 +631,6 @@
     <t xml:space="preserve">Strategic SAMs - Standoff Range </t>
   </si>
   <si>
-    <t>Precise location required</t>
-  </si>
-  <si>
     <t>SCLDD09</t>
   </si>
   <si>
@@ -1052,13 +1043,16 @@
   </si>
   <si>
     <t>F/A-18 Standard Conventional Loads</t>
+  </si>
+  <si>
+    <t>Standoff Cluster munitions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1571,7 +1565,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0B7C2BE-AA23-84B3-7AA4-502EE9479F26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0B7C2BE-AA23-84B3-7AA4-502EE9479F26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1583,7 +1577,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1621,7 +1615,7 @@
         <xdr:cNvPr id="7" name="Bilde 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90D77193-418F-9AEB-5548-3A3687C89635}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{90D77193-418F-9AEB-5548-3A3687C89635}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1633,7 +1627,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1675,7 +1669,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BED6E98-C195-4079-9F70-DD036F77C3D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BED6E98-C195-4079-9F70-DD036F77C3D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1687,7 +1681,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1725,7 +1719,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0115F003-202F-45B5-AC5E-0BAA43A3D433}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0115F003-202F-45B5-AC5E-0BAA43A3D433}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1737,7 +1731,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1779,7 +1773,7 @@
         <xdr:cNvPr id="2" name="Afbeelding 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC18912-9AA8-3425-780A-72F6F0C863A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBC18912-9AA8-3425-780A-72F6F0C863A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1788,10 +1782,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1811,7 +1805,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1840,7 +1834,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82B678FB-AB14-43CC-A68E-30E48EABF15B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82B678FB-AB14-43CC-A68E-30E48EABF15B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1852,7 +1846,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1890,7 +1884,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C512BEF4-7C0D-43BC-8A5B-CD9EAFD649AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C512BEF4-7C0D-43BC-8A5B-CD9EAFD649AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1902,7 +1896,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1944,7 +1938,7 @@
         <xdr:cNvPr id="3" name="Bilde 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEC48CA8-12AC-4465-9E3F-B9403871BC6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DEC48CA8-12AC-4465-9E3F-B9403871BC6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1956,7 +1950,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1994,7 +1988,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3472A29C-8552-4DC3-8E77-79AA30BA3A69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3472A29C-8552-4DC3-8E77-79AA30BA3A69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2006,7 +2000,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2048,7 +2042,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{291BB1BE-05A9-438D-9E42-D71A9373D6B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{291BB1BE-05A9-438D-9E42-D71A9373D6B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2060,7 +2054,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2098,7 +2092,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8534E27D-0272-47A0-A2AA-39CF4C41EC36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8534E27D-0272-47A0-A2AA-39CF4C41EC36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2110,7 +2104,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2175,7 +2169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2227,7 +2221,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2421,21 +2415,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262528F8-456E-4AF5-9CE6-DE707F112B84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.28515625" bestFit="1" customWidth="1"/>
@@ -2449,9 +2443,9 @@
     <col min="11" max="11" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:11" ht="61.5" x14ac:dyDescent="0.9">
+    <row r="6" spans="1:11" ht="61.5">
       <c r="A6" s="33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2464,31 +2458,31 @@
       <c r="J6" s="33"/>
       <c r="K6" s="33"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
         <v>265</v>
       </c>
-      <c r="B7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>266</v>
       </c>
-      <c r="B8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1">
       <c r="A9" t="s">
+        <v>268</v>
+      </c>
+      <c r="B9" t="s">
         <v>269</v>
       </c>
-      <c r="B9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -2514,7 +2508,7 @@
         <v>146</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>148</v>
@@ -2523,24 +2517,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>260</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>261</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>20</v>
@@ -2549,33 +2543,33 @@
         <v>10</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>20</v>
@@ -2584,31 +2578,31 @@
         <v>10</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>20</v>
@@ -2617,31 +2611,31 @@
         <v>10</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>276</v>
-      </c>
       <c r="F14" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>20</v>
@@ -2650,33 +2644,33 @@
         <v>10</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>20</v>
@@ -2685,31 +2679,31 @@
         <v>10</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>257</v>
-      </c>
       <c r="C16" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>20</v>
@@ -2718,40 +2712,40 @@
         <v>10</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>259</v>
-      </c>
       <c r="C17" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>10</v>
@@ -2769,14 +2763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC22DD4D-A328-4F2B-A934-70F281621B37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2786,9 +2780,9 @@
     <col min="9" max="9" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:9" ht="61.5" x14ac:dyDescent="0.9">
+    <row r="6" spans="1:9" ht="61.5">
       <c r="A6" s="33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2799,31 +2793,31 @@
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
         <v>265</v>
       </c>
-      <c r="B8" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>266</v>
       </c>
-      <c r="B9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
       <c r="A10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B10" t="s">
         <v>269</v>
       </c>
-      <c r="B10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -2846,39 +2840,39 @@
         <v>145</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>328</v>
-      </c>
       <c r="C12" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G12" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>330</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2891,14 +2885,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1781B9E3-0467-4D07-A3EF-242542BBC216}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
@@ -2910,9 +2904,9 @@
     <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:13" ht="61.5" x14ac:dyDescent="0.9">
+    <row r="6" spans="1:13" ht="61.5">
       <c r="A6" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2927,567 +2921,567 @@
       <c r="L6" s="33"/>
       <c r="M6" s="33"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="9" spans="1:13" ht="16.5" thickBot="1">
       <c r="A9" s="18"/>
       <c r="B9" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A10" s="20" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="C10" s="21" t="s">
         <v>283</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>284</v>
       </c>
       <c r="D10" s="21">
         <v>7</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F10" s="21">
         <v>2</v>
       </c>
       <c r="G10" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="H10" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="H10" s="22" t="s">
+    </row>
+    <row r="11" spans="1:13" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A11" s="23" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="B11" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="C11" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="E11" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="F11" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="G11" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A12" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="B12" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="D12" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="E12" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="F12" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="G12" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A13" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="E13" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="B12" s="27" t="s">
+    </row>
+    <row r="14" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A14" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A15" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E12" s="27" t="s">
+      <c r="D15" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="F12" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="H12" s="28" t="s">
+      <c r="E15" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A16" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A17" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="D17" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A18" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>294</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="D18" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A19" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E13" s="24" t="s">
+      <c r="D19" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="H13" s="25" t="s">
+      <c r="E19" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G19" s="24" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+      <c r="H19" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A20" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A21" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A22" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C22" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="D22" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>309</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A23" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A24" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A25" s="23" t="s">
+        <v>314</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A26" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A27" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A28" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A29" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="G29" s="24" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E14" s="27" t="s">
+      <c r="H29" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="16.5" thickBot="1">
+      <c r="A30" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="D30" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="F14" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E15" s="24" t="s">
+      <c r="E30" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="F30" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="F15" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="H16" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>301</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
-        <v>303</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>304</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26" t="s">
-        <v>305</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>306</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G20" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
-        <v>307</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
-        <v>309</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G22" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
-        <v>311</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="H24" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
-        <v>315</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>316</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>318</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G26" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="H26" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
-        <v>319</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>320</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E28" s="27" t="s">
-        <v>322</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="G28" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="H28" s="28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23" t="s">
-        <v>323</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>324</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="H29" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
-        <v>325</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>326</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>290</v>
-      </c>
       <c r="G30" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3501,14 +3495,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B9F48F-DC77-443E-BB86-F83AD97118A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
@@ -3520,7 +3514,7 @@
     <col min="11" max="11" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="12.75" customHeight="1">
       <c r="A1" s="15"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -3533,25 +3527,25 @@
       <c r="J1" s="16"/>
       <c r="K1" s="17"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="1"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="61.5" x14ac:dyDescent="0.9">
+    <row r="6" spans="1:11" ht="61.5">
       <c r="A6" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -3564,18 +3558,18 @@
       <c r="J6" s="33"/>
       <c r="K6" s="35"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="1"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="1"/>
       <c r="C8" t="s">
         <v>136</v>
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="1"/>
       <c r="C9" t="s">
         <v>137</v>
@@ -3585,25 +3579,25 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="1"/>
       <c r="C10" t="s">
         <v>139</v>
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="1"/>
       <c r="C11" t="s">
         <v>140</v>
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1">
       <c r="A12" s="1"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -3638,7 +3632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="30" t="s">
         <v>149</v>
       </c>
@@ -3671,7 +3665,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="31" t="s">
         <v>156</v>
       </c>
@@ -3704,7 +3698,7 @@
       </c>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="31" t="s">
         <v>158</v>
       </c>
@@ -3737,7 +3731,7 @@
       </c>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="31" t="s">
         <v>159</v>
       </c>
@@ -3770,7 +3764,7 @@
       </c>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="31" t="s">
         <v>161</v>
       </c>
@@ -3803,7 +3797,7 @@
       </c>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="31" t="s">
         <v>163</v>
       </c>
@@ -3836,7 +3830,7 @@
       </c>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="31" t="s">
         <v>166</v>
       </c>
@@ -3869,7 +3863,7 @@
       </c>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="31" t="s">
         <v>168</v>
       </c>
@@ -3902,7 +3896,7 @@
       </c>
       <c r="K21" s="11"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="31" t="s">
         <v>170</v>
       </c>
@@ -3935,7 +3929,7 @@
       </c>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="31" t="s">
         <v>172</v>
       </c>
@@ -3968,7 +3962,7 @@
       </c>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="31" t="s">
         <v>174</v>
       </c>
@@ -4001,7 +3995,7 @@
       </c>
       <c r="K24" s="11"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="31" t="s">
         <v>176</v>
       </c>
@@ -4034,7 +4028,7 @@
       </c>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="32" t="s">
         <v>178</v>
       </c>
@@ -4067,7 +4061,7 @@
       </c>
       <c r="K26" s="14"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="30" t="s">
         <v>180</v>
       </c>
@@ -4100,7 +4094,7 @@
       </c>
       <c r="K27" s="8"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="31" t="s">
         <v>183</v>
       </c>
@@ -4133,7 +4127,7 @@
       </c>
       <c r="K28" s="11"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="31" t="s">
         <v>186</v>
       </c>
@@ -4166,7 +4160,7 @@
       </c>
       <c r="K29" s="11"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1">
       <c r="A30" s="32" t="s">
         <v>188</v>
       </c>
@@ -4199,7 +4193,7 @@
       </c>
       <c r="K30" s="14"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="30" t="s">
         <v>190</v>
       </c>
@@ -4232,7 +4226,7 @@
       </c>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="31" t="s">
         <v>192</v>
       </c>
@@ -4265,7 +4259,7 @@
       </c>
       <c r="K32" s="11"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="31" t="s">
         <v>193</v>
       </c>
@@ -4298,7 +4292,7 @@
       </c>
       <c r="K33" s="11"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="31" t="s">
         <v>194</v>
       </c>
@@ -4331,7 +4325,7 @@
       </c>
       <c r="K34" s="11"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="31" t="s">
         <v>195</v>
       </c>
@@ -4364,7 +4358,7 @@
       </c>
       <c r="K35" s="11"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="31" t="s">
         <v>196</v>
       </c>
@@ -4397,7 +4391,7 @@
       </c>
       <c r="K36" s="11"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="31" t="s">
         <v>197</v>
       </c>
@@ -4430,7 +4424,7 @@
       </c>
       <c r="K37" s="11"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="31" t="s">
         <v>198</v>
       </c>
@@ -4462,12 +4456,12 @@
         <v>148</v>
       </c>
       <c r="K38" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A39" s="32" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="32" t="s">
-        <v>201</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>52</v>
@@ -4479,7 +4473,7 @@
         <v>10</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>182</v>
@@ -4496,25 +4490,25 @@
       <c r="J39" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="K39" s="14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>69</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>182</v>
@@ -4532,18 +4526,18 @@
         <v>155</v>
       </c>
       <c r="K40" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="31" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
-        <v>207</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>20</v>
@@ -4567,24 +4561,24 @@
         <v>155</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>182</v>
@@ -4602,24 +4596,24 @@
         <v>155</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>182</v>
@@ -4637,18 +4631,18 @@
         <v>155</v>
       </c>
       <c r="K43" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="31" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
-        <v>213</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>10</v>
@@ -4672,18 +4666,18 @@
         <v>155</v>
       </c>
       <c r="K44" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="31" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
-        <v>215</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>10</v>
@@ -4707,18 +4701,18 @@
         <v>155</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>10</v>
@@ -4742,18 +4736,18 @@
         <v>155</v>
       </c>
       <c r="K46" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="31" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
-        <v>218</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>10</v>
@@ -4777,24 +4771,24 @@
         <v>155</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>182</v>
@@ -4812,18 +4806,18 @@
         <v>155</v>
       </c>
       <c r="K48" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="31" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
-        <v>222</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>10</v>
@@ -4847,18 +4841,18 @@
         <v>155</v>
       </c>
       <c r="K49" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="31" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
-        <v>224</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>10</v>
@@ -4882,24 +4876,24 @@
         <v>155</v>
       </c>
       <c r="K50" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A51" s="32" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="32" t="s">
-        <v>226</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F51" s="13" t="s">
         <v>182</v>
@@ -4917,24 +4911,24 @@
         <v>155</v>
       </c>
       <c r="K51" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="30" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
-        <v>229</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F52" s="7">
         <v>600</v>
@@ -4953,27 +4947,27 @@
       </c>
       <c r="K52" s="8"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>110</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F53" s="10">
         <v>600</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>153</v>
@@ -4985,24 +4979,24 @@
         <v>20</v>
       </c>
       <c r="K53" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="31" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
-        <v>235</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>110</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F54" s="10">
         <v>402</v>
@@ -5021,27 +5015,27 @@
       </c>
       <c r="K54" s="11"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>110</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F55" s="10">
         <v>402</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>153</v>
@@ -5053,30 +5047,30 @@
         <v>20</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" thickBot="1">
       <c r="A56" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>110</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F56" s="13">
         <v>600</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>153</v>
@@ -5089,21 +5083,21 @@
       </c>
       <c r="K56" s="14"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>242</v>
-      </c>
       <c r="C57" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F57" s="7">
         <v>501</v>
@@ -5122,27 +5116,27 @@
       </c>
       <c r="K57" s="8"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="A58" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F58" s="10">
         <v>501</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>153</v>
@@ -5154,24 +5148,24 @@
         <v>20</v>
       </c>
       <c r="K58" s="11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F59" s="10">
         <v>402</v>
@@ -5190,27 +5184,27 @@
       </c>
       <c r="K59" s="11"/>
     </row>
-    <row r="60" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="15.75" thickBot="1">
       <c r="A60" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F60" s="13">
         <v>402</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>153</v>
@@ -5222,7 +5216,7 @@
         <v>20</v>
       </c>
       <c r="K60" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -5236,14 +5230,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8A92FB-D007-46A8-ADB3-52391952E704}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
@@ -5255,9 +5249,9 @@
     <col min="9" max="9" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:9" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" ht="36">
       <c r="A6" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
@@ -5268,8 +5262,8 @@
       <c r="H6" s="36"/>
       <c r="I6" s="36"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -5298,7 +5292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="30" t="s">
         <v>7</v>
       </c>
@@ -5327,7 +5321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="31" t="s">
         <v>14</v>
       </c>
@@ -5356,7 +5350,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="31" t="s">
         <v>15</v>
       </c>
@@ -5385,7 +5379,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="31" t="s">
         <v>18</v>
       </c>
@@ -5414,7 +5408,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="31" t="s">
         <v>19</v>
       </c>
@@ -5443,7 +5437,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="31" t="s">
         <v>23</v>
       </c>
@@ -5472,7 +5466,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.75" thickBot="1">
       <c r="A15" s="32" t="s">
         <v>24</v>
       </c>
@@ -5501,7 +5495,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="30" t="s">
         <v>25</v>
       </c>
@@ -5528,7 +5522,7 @@
       </c>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="31" t="s">
         <v>35</v>
       </c>
@@ -5557,7 +5551,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="31" t="s">
         <v>38</v>
       </c>
@@ -5584,7 +5578,7 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="31" t="s">
         <v>49</v>
       </c>
@@ -5611,7 +5605,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="31" t="s">
         <v>98</v>
       </c>
@@ -5638,7 +5632,7 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="31" t="s">
         <v>101</v>
       </c>
@@ -5665,7 +5659,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1">
       <c r="A22" s="32" t="s">
         <v>104</v>
       </c>
@@ -5692,7 +5686,7 @@
       </c>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="30" t="s">
         <v>51</v>
       </c>
@@ -5719,7 +5713,7 @@
       </c>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="31" t="s">
         <v>53</v>
       </c>
@@ -5748,7 +5742,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="31" t="s">
         <v>59</v>
       </c>
@@ -5775,7 +5769,7 @@
       </c>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="31" t="s">
         <v>60</v>
       </c>
@@ -5804,7 +5798,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="31" t="s">
         <v>63</v>
       </c>
@@ -5833,7 +5827,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1">
       <c r="A28" s="32" t="s">
         <v>64</v>
       </c>
@@ -5862,7 +5856,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="30" t="s">
         <v>68</v>
       </c>
@@ -5891,7 +5885,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="31" t="s">
         <v>72</v>
       </c>
@@ -5920,7 +5914,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="31" t="s">
         <v>74</v>
       </c>
@@ -5949,7 +5943,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="31" t="s">
         <v>76</v>
       </c>
@@ -5978,7 +5972,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="31" t="s">
         <v>78</v>
       </c>
@@ -6007,7 +6001,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="31" t="s">
         <v>79</v>
       </c>
@@ -6036,7 +6030,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="31" t="s">
         <v>80</v>
       </c>
@@ -6065,7 +6059,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="31" t="s">
         <v>85</v>
       </c>
@@ -6094,7 +6088,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="31" t="s">
         <v>86</v>
       </c>
@@ -6123,7 +6117,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="31" t="s">
         <v>87</v>
       </c>
@@ -6152,7 +6146,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="31" t="s">
         <v>90</v>
       </c>
@@ -6181,7 +6175,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15.75" thickBot="1">
       <c r="A40" s="32" t="s">
         <v>107</v>
       </c>
@@ -6210,7 +6204,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="30" t="s">
         <v>117</v>
       </c>
@@ -6239,7 +6233,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="31" t="s">
         <v>118</v>
       </c>
@@ -6268,7 +6262,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="31" t="s">
         <v>119</v>
       </c>
@@ -6295,7 +6289,7 @@
       </c>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="31" t="s">
         <v>120</v>
       </c>
@@ -6324,7 +6318,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15.75" thickBot="1">
       <c r="A45" s="32" t="s">
         <v>121</v>
       </c>
@@ -6353,7 +6347,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="30" t="s">
         <v>122</v>
       </c>
@@ -6380,7 +6374,7 @@
       </c>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="31" t="s">
         <v>124</v>
       </c>
@@ -6407,7 +6401,7 @@
       </c>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15.75" thickBot="1">
       <c r="A48" s="32" t="s">
         <v>125</v>
       </c>
@@ -6436,7 +6430,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="30" t="s">
         <v>126</v>
       </c>
@@ -6463,7 +6457,7 @@
       </c>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="31" t="s">
         <v>130</v>
       </c>
@@ -6492,7 +6486,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15.75" thickBot="1">
       <c r="A51" s="32" t="s">
         <v>133</v>
       </c>

</xml_diff>